<commit_message>
v4.2.8 support baker programming
1. add test function for baker programming
</commit_message>
<xml_diff>
--- a/SenkoMicro-SKCS-GUI - auto/Programming Discription/LABtest_公式_v1.2 (自动保存的).xlsx
+++ b/SenkoMicro-SKCS-GUI - auto/Programming Discription/LABtest_公式_v1.2 (自动保存的).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="1185" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="实验室测试项目" sheetId="7" r:id="rId1"/>
@@ -3040,6 +3040,99 @@
     <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3112,12 +3205,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3126,93 +3213,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4050,11 +4050,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="290763680"/>
-        <c:axId val="290764240"/>
+        <c:axId val="200488000"/>
+        <c:axId val="200488560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290763680"/>
+        <c:axId val="200488000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4063,7 +4063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290764240"/>
+        <c:crossAx val="200488560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4071,7 +4071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290764240"/>
+        <c:axId val="200488560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4082,7 +4082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290763680"/>
+        <c:crossAx val="200488000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4523,11 +4523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="291967232"/>
-        <c:axId val="291967792"/>
+        <c:axId val="201141408"/>
+        <c:axId val="201141968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="291967232"/>
+        <c:axId val="201141408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4536,7 +4536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291967792"/>
+        <c:crossAx val="201141968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4544,7 +4544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291967792"/>
+        <c:axId val="201141968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4555,7 +4555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291967232"/>
+        <c:crossAx val="201141408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4996,11 +4996,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="291973392"/>
-        <c:axId val="291973952"/>
+        <c:axId val="201306224"/>
+        <c:axId val="201306784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="291973392"/>
+        <c:axId val="201306224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5009,7 +5009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291973952"/>
+        <c:crossAx val="201306784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5017,7 +5017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="291973952"/>
+        <c:axId val="201306784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,13 +5028,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291973392"/>
+        <c:crossAx val="201306224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5482,11 +5483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="292170864"/>
-        <c:axId val="292171424"/>
+        <c:axId val="201335232"/>
+        <c:axId val="201335792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="292170864"/>
+        <c:axId val="201335232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5495,7 +5496,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292171424"/>
+        <c:crossAx val="201335792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5503,7 +5504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292171424"/>
+        <c:axId val="201335792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5518,7 +5519,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292170864"/>
+        <c:crossAx val="201335232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5645,11 +5646,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="292174784"/>
-        <c:axId val="292175344"/>
+        <c:axId val="201468176"/>
+        <c:axId val="201468736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="292174784"/>
+        <c:axId val="201468176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5692,7 +5693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292175344"/>
+        <c:crossAx val="201468736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5700,7 +5701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292175344"/>
+        <c:axId val="201468736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5751,7 +5752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="292174784"/>
+        <c:crossAx val="201468176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6827,50 +6828,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="48" customHeight="1" thickBot="1">
-      <c r="A1" s="635" t="s">
+      <c r="A1" s="666" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="636"/>
-      <c r="C1" s="636"/>
-      <c r="D1" s="636"/>
-      <c r="E1" s="636"/>
-      <c r="F1" s="636"/>
-      <c r="G1" s="636"/>
-      <c r="H1" s="636"/>
-      <c r="I1" s="636"/>
-      <c r="J1" s="636"/>
-      <c r="K1" s="636"/>
-      <c r="L1" s="637"/>
+      <c r="B1" s="667"/>
+      <c r="C1" s="667"/>
+      <c r="D1" s="667"/>
+      <c r="E1" s="667"/>
+      <c r="F1" s="667"/>
+      <c r="G1" s="667"/>
+      <c r="H1" s="667"/>
+      <c r="I1" s="667"/>
+      <c r="J1" s="667"/>
+      <c r="K1" s="667"/>
+      <c r="L1" s="668"/>
     </row>
     <row r="2" spans="1:12" ht="39" customHeight="1" thickBot="1">
-      <c r="A2" s="649"/>
-      <c r="B2" s="649"/>
-      <c r="C2" s="649"/>
-      <c r="D2" s="649"/>
-      <c r="E2" s="649"/>
-      <c r="F2" s="649"/>
-      <c r="G2" s="649"/>
-      <c r="H2" s="649"/>
-      <c r="I2" s="649"/>
-      <c r="J2" s="649"/>
-      <c r="K2" s="649"/>
-      <c r="L2" s="649"/>
+      <c r="A2" s="680"/>
+      <c r="B2" s="680"/>
+      <c r="C2" s="680"/>
+      <c r="D2" s="680"/>
+      <c r="E2" s="680"/>
+      <c r="F2" s="680"/>
+      <c r="G2" s="680"/>
+      <c r="H2" s="680"/>
+      <c r="I2" s="680"/>
+      <c r="J2" s="680"/>
+      <c r="K2" s="680"/>
+      <c r="L2" s="680"/>
     </row>
     <row r="3" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A3" s="661" t="s">
+      <c r="A3" s="690" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="662"/>
-      <c r="C3" s="662"/>
-      <c r="D3" s="662"/>
-      <c r="E3" s="662"/>
-      <c r="F3" s="662"/>
-      <c r="G3" s="662"/>
-      <c r="H3" s="662"/>
-      <c r="I3" s="662"/>
-      <c r="J3" s="662"/>
-      <c r="K3" s="662"/>
-      <c r="L3" s="663"/>
+      <c r="B3" s="691"/>
+      <c r="C3" s="691"/>
+      <c r="D3" s="691"/>
+      <c r="E3" s="691"/>
+      <c r="F3" s="691"/>
+      <c r="G3" s="691"/>
+      <c r="H3" s="691"/>
+      <c r="I3" s="691"/>
+      <c r="J3" s="691"/>
+      <c r="K3" s="691"/>
+      <c r="L3" s="692"/>
     </row>
     <row r="4" spans="1:12" ht="89.25" customHeight="1" thickBot="1">
       <c r="A4" s="151" t="s">
@@ -6891,11 +6892,11 @@
       <c r="F4" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="638" t="s">
+      <c r="G4" s="669" t="s">
         <v>163</v>
       </c>
-      <c r="H4" s="638"/>
-      <c r="I4" s="638"/>
+      <c r="H4" s="669"/>
+      <c r="I4" s="669"/>
       <c r="J4" s="155" t="s">
         <v>164</v>
       </c>
@@ -6903,21 +6904,21 @@
       <c r="L4" s="16"/>
     </row>
     <row r="5" spans="1:12" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A5" s="650"/>
-      <c r="B5" s="651"/>
-      <c r="C5" s="651"/>
-      <c r="D5" s="651"/>
-      <c r="E5" s="651"/>
-      <c r="F5" s="651"/>
-      <c r="G5" s="651"/>
-      <c r="H5" s="651"/>
-      <c r="I5" s="651"/>
-      <c r="J5" s="651"/>
-      <c r="K5" s="651"/>
-      <c r="L5" s="652"/>
+      <c r="A5" s="681"/>
+      <c r="B5" s="682"/>
+      <c r="C5" s="682"/>
+      <c r="D5" s="682"/>
+      <c r="E5" s="682"/>
+      <c r="F5" s="682"/>
+      <c r="G5" s="682"/>
+      <c r="H5" s="682"/>
+      <c r="I5" s="682"/>
+      <c r="J5" s="682"/>
+      <c r="K5" s="682"/>
+      <c r="L5" s="683"/>
     </row>
     <row r="6" spans="1:12" ht="15.75">
-      <c r="A6" s="639">
+      <c r="A6" s="670">
         <v>1</v>
       </c>
       <c r="B6" s="86" t="s">
@@ -6938,7 +6939,7 @@
       <c r="G6" s="88">
         <v>5.5</v>
       </c>
-      <c r="H6" s="676" t="s">
+      <c r="H6" s="639" t="s">
         <v>165</v>
       </c>
       <c r="I6" s="90"/>
@@ -6947,7 +6948,7 @@
       <c r="L6" s="170"/>
     </row>
     <row r="7" spans="1:12" ht="15.75">
-      <c r="A7" s="640"/>
+      <c r="A7" s="671"/>
       <c r="B7" s="91" t="s">
         <v>31</v>
       </c>
@@ -6956,14 +6957,14 @@
       <c r="E7" s="93"/>
       <c r="F7" s="94"/>
       <c r="G7" s="95"/>
-      <c r="H7" s="676"/>
+      <c r="H7" s="639"/>
       <c r="I7" s="90"/>
       <c r="J7" s="90"/>
       <c r="K7" s="90"/>
       <c r="L7" s="170"/>
     </row>
     <row r="8" spans="1:12" ht="15.75">
-      <c r="A8" s="640"/>
+      <c r="A8" s="671"/>
       <c r="B8" s="91" t="s">
         <v>32</v>
       </c>
@@ -6972,14 +6973,14 @@
       <c r="E8" s="166"/>
       <c r="F8" s="96"/>
       <c r="G8" s="97"/>
-      <c r="H8" s="676"/>
+      <c r="H8" s="639"/>
       <c r="I8" s="98"/>
       <c r="J8" s="98"/>
       <c r="K8" s="98"/>
       <c r="L8" s="171"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A9" s="641"/>
+      <c r="A9" s="672"/>
       <c r="B9" s="99" t="s">
         <v>33</v>
       </c>
@@ -6988,28 +6989,28 @@
       <c r="E9" s="101"/>
       <c r="F9" s="100"/>
       <c r="G9" s="102"/>
-      <c r="H9" s="676"/>
+      <c r="H9" s="639"/>
       <c r="I9" s="89"/>
       <c r="J9" s="89"/>
       <c r="K9" s="89"/>
       <c r="L9" s="170"/>
     </row>
     <row r="10" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A10" s="653"/>
-      <c r="B10" s="654"/>
-      <c r="C10" s="654"/>
-      <c r="D10" s="654"/>
-      <c r="E10" s="654"/>
-      <c r="F10" s="654"/>
-      <c r="G10" s="654"/>
-      <c r="H10" s="654"/>
-      <c r="I10" s="655"/>
-      <c r="J10" s="655"/>
-      <c r="K10" s="655"/>
-      <c r="L10" s="656"/>
+      <c r="A10" s="684"/>
+      <c r="B10" s="685"/>
+      <c r="C10" s="685"/>
+      <c r="D10" s="685"/>
+      <c r="E10" s="685"/>
+      <c r="F10" s="685"/>
+      <c r="G10" s="685"/>
+      <c r="H10" s="685"/>
+      <c r="I10" s="686"/>
+      <c r="J10" s="686"/>
+      <c r="K10" s="686"/>
+      <c r="L10" s="687"/>
     </row>
     <row r="11" spans="1:12" ht="72.75" customHeight="1">
-      <c r="A11" s="646">
+      <c r="A11" s="677">
         <v>2</v>
       </c>
       <c r="B11" s="103" t="s">
@@ -7031,7 +7032,7 @@
         <v>96</v>
       </c>
       <c r="H11" s="105"/>
-      <c r="I11" s="676" t="s">
+      <c r="I11" s="639" t="s">
         <v>170</v>
       </c>
       <c r="J11" s="89"/>
@@ -7039,11 +7040,11 @@
       <c r="L11" s="172"/>
     </row>
     <row r="12" spans="1:12" ht="15.75">
-      <c r="A12" s="647"/>
-      <c r="B12" s="659">
-        <v>1</v>
-      </c>
-      <c r="C12" s="659">
+      <c r="A12" s="678"/>
+      <c r="B12" s="648">
+        <v>1</v>
+      </c>
+      <c r="C12" s="648">
         <v>1</v>
       </c>
       <c r="D12" s="106">
@@ -7055,15 +7056,15 @@
       <c r="F12" s="93"/>
       <c r="G12" s="93"/>
       <c r="H12" s="108"/>
-      <c r="I12" s="676"/>
+      <c r="I12" s="639"/>
       <c r="J12" s="109"/>
       <c r="K12" s="109"/>
       <c r="L12" s="173"/>
     </row>
     <row r="13" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A13" s="647"/>
-      <c r="B13" s="659"/>
-      <c r="C13" s="659"/>
+      <c r="A13" s="678"/>
+      <c r="B13" s="648"/>
+      <c r="C13" s="648"/>
       <c r="D13" s="106">
         <v>0</v>
       </c>
@@ -7073,15 +7074,15 @@
       <c r="F13" s="94"/>
       <c r="G13" s="94"/>
       <c r="H13" s="95"/>
-      <c r="I13" s="676"/>
+      <c r="I13" s="639"/>
       <c r="J13" s="90"/>
       <c r="K13" s="90"/>
       <c r="L13" s="170"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
-      <c r="A14" s="647"/>
-      <c r="B14" s="659"/>
-      <c r="C14" s="659"/>
+      <c r="A14" s="678"/>
+      <c r="B14" s="648"/>
+      <c r="C14" s="648"/>
       <c r="D14" s="106">
         <v>1</v>
       </c>
@@ -7091,15 +7092,15 @@
       <c r="F14" s="94"/>
       <c r="G14" s="94"/>
       <c r="H14" s="95"/>
-      <c r="I14" s="676"/>
+      <c r="I14" s="639"/>
       <c r="J14" s="90"/>
       <c r="K14" s="90"/>
       <c r="L14" s="170"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A15" s="648"/>
-      <c r="B15" s="660"/>
-      <c r="C15" s="660"/>
+      <c r="A15" s="679"/>
+      <c r="B15" s="649"/>
+      <c r="C15" s="649"/>
       <c r="D15" s="100">
         <v>1</v>
       </c>
@@ -7109,36 +7110,36 @@
       <c r="F15" s="111"/>
       <c r="G15" s="111"/>
       <c r="H15" s="112"/>
-      <c r="I15" s="676"/>
+      <c r="I15" s="639"/>
       <c r="J15" s="90"/>
       <c r="K15" s="90"/>
       <c r="L15" s="170"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A16" s="647"/>
-      <c r="B16" s="657"/>
-      <c r="C16" s="657"/>
-      <c r="D16" s="657"/>
-      <c r="E16" s="657"/>
-      <c r="F16" s="657"/>
-      <c r="G16" s="657"/>
-      <c r="H16" s="657"/>
-      <c r="I16" s="657"/>
-      <c r="J16" s="657"/>
-      <c r="K16" s="657"/>
-      <c r="L16" s="658"/>
+      <c r="A16" s="678"/>
+      <c r="B16" s="688"/>
+      <c r="C16" s="688"/>
+      <c r="D16" s="688"/>
+      <c r="E16" s="688"/>
+      <c r="F16" s="688"/>
+      <c r="G16" s="688"/>
+      <c r="H16" s="688"/>
+      <c r="I16" s="688"/>
+      <c r="J16" s="688"/>
+      <c r="K16" s="688"/>
+      <c r="L16" s="689"/>
     </row>
     <row r="17" spans="1:12" ht="15.75">
-      <c r="A17" s="642">
+      <c r="A17" s="673">
         <v>3</v>
       </c>
       <c r="B17" s="103" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="645" t="s">
+      <c r="C17" s="676" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="645"/>
+      <c r="D17" s="676"/>
       <c r="E17" s="64" t="s">
         <v>34</v>
       </c>
@@ -7158,19 +7159,19 @@
         <v>5.5</v>
       </c>
       <c r="K17" s="84"/>
-      <c r="L17" s="677" t="s">
+      <c r="L17" s="640" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="643"/>
-      <c r="B18" s="659">
-        <v>0</v>
-      </c>
-      <c r="C18" s="659">
-        <v>1</v>
-      </c>
-      <c r="D18" s="659"/>
+      <c r="A18" s="674"/>
+      <c r="B18" s="648">
+        <v>0</v>
+      </c>
+      <c r="C18" s="648">
+        <v>1</v>
+      </c>
+      <c r="D18" s="648"/>
       <c r="E18" s="59" t="s">
         <v>36</v>
       </c>
@@ -7180,13 +7181,13 @@
       <c r="I18" s="93"/>
       <c r="J18" s="93"/>
       <c r="K18" s="108"/>
-      <c r="L18" s="677"/>
+      <c r="L18" s="640"/>
     </row>
     <row r="19" spans="1:12" ht="15.75">
-      <c r="A19" s="643"/>
-      <c r="B19" s="659"/>
-      <c r="C19" s="659"/>
-      <c r="D19" s="659"/>
+      <c r="A19" s="674"/>
+      <c r="B19" s="648"/>
+      <c r="C19" s="648"/>
+      <c r="D19" s="648"/>
       <c r="E19" s="59" t="s">
         <v>37</v>
       </c>
@@ -7196,13 +7197,13 @@
       <c r="I19" s="93"/>
       <c r="J19" s="93"/>
       <c r="K19" s="108"/>
-      <c r="L19" s="677"/>
+      <c r="L19" s="640"/>
     </row>
     <row r="20" spans="1:12" ht="15.75">
-      <c r="A20" s="643"/>
-      <c r="B20" s="659"/>
-      <c r="C20" s="659"/>
-      <c r="D20" s="659"/>
+      <c r="A20" s="674"/>
+      <c r="B20" s="648"/>
+      <c r="C20" s="648"/>
+      <c r="D20" s="648"/>
       <c r="E20" s="59" t="s">
         <v>38</v>
       </c>
@@ -7212,13 +7213,13 @@
       <c r="I20" s="93"/>
       <c r="J20" s="93"/>
       <c r="K20" s="108"/>
-      <c r="L20" s="677"/>
+      <c r="L20" s="640"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A21" s="644"/>
-      <c r="B21" s="660"/>
-      <c r="C21" s="660"/>
-      <c r="D21" s="660"/>
+      <c r="A21" s="675"/>
+      <c r="B21" s="649"/>
+      <c r="C21" s="649"/>
+      <c r="D21" s="649"/>
       <c r="E21" s="85" t="s">
         <v>35</v>
       </c>
@@ -7243,24 +7244,24 @@
         <v>0</v>
       </c>
       <c r="K21" s="114"/>
-      <c r="L21" s="677"/>
+      <c r="L21" s="640"/>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A22" s="672"/>
-      <c r="B22" s="673"/>
-      <c r="C22" s="673"/>
-      <c r="D22" s="673"/>
-      <c r="E22" s="673"/>
-      <c r="F22" s="673"/>
-      <c r="G22" s="673"/>
-      <c r="H22" s="673"/>
-      <c r="I22" s="673"/>
-      <c r="J22" s="673"/>
-      <c r="K22" s="673"/>
-      <c r="L22" s="674"/>
+      <c r="A22" s="635"/>
+      <c r="B22" s="636"/>
+      <c r="C22" s="636"/>
+      <c r="D22" s="636"/>
+      <c r="E22" s="636"/>
+      <c r="F22" s="636"/>
+      <c r="G22" s="636"/>
+      <c r="H22" s="636"/>
+      <c r="I22" s="636"/>
+      <c r="J22" s="636"/>
+      <c r="K22" s="636"/>
+      <c r="L22" s="637"/>
     </row>
     <row r="23" spans="1:12" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A23" s="665">
+      <c r="A23" s="660">
         <v>4</v>
       </c>
       <c r="B23" s="161" t="s">
@@ -7290,7 +7291,7 @@
       <c r="L23" s="174"/>
     </row>
     <row r="24" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A24" s="666"/>
+      <c r="A24" s="661"/>
       <c r="B24" s="162">
         <v>0</v>
       </c>
@@ -7307,13 +7308,13 @@
       </c>
       <c r="I24" s="93"/>
       <c r="J24" s="108"/>
-      <c r="K24" s="678" t="s">
+      <c r="K24" s="641" t="s">
         <v>172</v>
       </c>
       <c r="L24" s="174"/>
     </row>
     <row r="25" spans="1:12" ht="18" customHeight="1">
-      <c r="A25" s="666"/>
+      <c r="A25" s="661"/>
       <c r="B25" s="162">
         <v>0</v>
       </c>
@@ -7330,11 +7331,11 @@
       </c>
       <c r="I25" s="93"/>
       <c r="J25" s="108"/>
-      <c r="K25" s="678"/>
+      <c r="K25" s="641"/>
       <c r="L25" s="174"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="A26" s="666"/>
+      <c r="A26" s="661"/>
       <c r="B26" s="162">
         <v>1</v>
       </c>
@@ -7351,11 +7352,11 @@
       </c>
       <c r="I26" s="93"/>
       <c r="J26" s="108"/>
-      <c r="K26" s="678"/>
+      <c r="K26" s="641"/>
       <c r="L26" s="174"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A27" s="667"/>
+      <c r="A27" s="662"/>
       <c r="B27" s="163">
         <v>1</v>
       </c>
@@ -7372,7 +7373,7 @@
       </c>
       <c r="I27" s="113"/>
       <c r="J27" s="114"/>
-      <c r="K27" s="678"/>
+      <c r="K27" s="641"/>
       <c r="L27" s="175"/>
     </row>
     <row r="28" spans="1:12" ht="18.75" customHeight="1">
@@ -7390,7 +7391,7 @@
       <c r="L28" s="175"/>
     </row>
     <row r="29" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A29" s="669">
+      <c r="A29" s="655">
         <v>5</v>
       </c>
       <c r="B29" s="106" t="s">
@@ -7406,7 +7407,7 @@
         <v>174</v>
       </c>
       <c r="F29" s="160"/>
-      <c r="G29" s="670" t="s">
+      <c r="G29" s="664" t="s">
         <v>175</v>
       </c>
       <c r="H29" s="109"/>
@@ -7416,8 +7417,8 @@
       <c r="L29" s="175"/>
     </row>
     <row r="30" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A30" s="669"/>
-      <c r="B30" s="668">
+      <c r="A30" s="655"/>
+      <c r="B30" s="663">
         <v>1</v>
       </c>
       <c r="C30" s="107">
@@ -7426,7 +7427,7 @@
       <c r="D30" s="164"/>
       <c r="E30" s="165"/>
       <c r="F30" s="160"/>
-      <c r="G30" s="670"/>
+      <c r="G30" s="664"/>
       <c r="H30" s="109"/>
       <c r="I30" s="160"/>
       <c r="J30" s="160"/>
@@ -7434,15 +7435,15 @@
       <c r="L30" s="175"/>
     </row>
     <row r="31" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A31" s="669"/>
-      <c r="B31" s="668"/>
+      <c r="A31" s="655"/>
+      <c r="B31" s="663"/>
       <c r="C31" s="107">
         <v>1</v>
       </c>
       <c r="D31" s="164"/>
       <c r="E31" s="165"/>
       <c r="F31" s="160"/>
-      <c r="G31" s="670"/>
+      <c r="G31" s="664"/>
       <c r="H31" s="109"/>
       <c r="I31" s="160"/>
       <c r="J31" s="160"/>
@@ -7450,50 +7451,50 @@
       <c r="L31" s="175"/>
     </row>
     <row r="32" spans="1:12" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A32" s="680" t="s">
+      <c r="A32" s="643" t="s">
         <v>176</v>
       </c>
-      <c r="B32" s="679"/>
-      <c r="C32" s="679"/>
-      <c r="D32" s="679"/>
-      <c r="E32" s="679"/>
-      <c r="F32" s="679"/>
-      <c r="G32" s="679"/>
-      <c r="H32" s="679"/>
-      <c r="I32" s="679"/>
-      <c r="J32" s="679"/>
-      <c r="K32" s="679"/>
-      <c r="L32" s="681"/>
+      <c r="B32" s="642"/>
+      <c r="C32" s="642"/>
+      <c r="D32" s="642"/>
+      <c r="E32" s="642"/>
+      <c r="F32" s="642"/>
+      <c r="G32" s="642"/>
+      <c r="H32" s="642"/>
+      <c r="I32" s="642"/>
+      <c r="J32" s="642"/>
+      <c r="K32" s="642"/>
+      <c r="L32" s="644"/>
     </row>
     <row r="33" spans="1:31" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A33" s="679"/>
-      <c r="B33" s="679"/>
-      <c r="C33" s="679"/>
-      <c r="D33" s="679"/>
-      <c r="E33" s="679"/>
-      <c r="F33" s="679"/>
-      <c r="G33" s="679"/>
-      <c r="H33" s="679"/>
-      <c r="I33" s="679"/>
-      <c r="J33" s="679"/>
-      <c r="K33" s="679"/>
-      <c r="L33" s="679"/>
+      <c r="A33" s="642"/>
+      <c r="B33" s="642"/>
+      <c r="C33" s="642"/>
+      <c r="D33" s="642"/>
+      <c r="E33" s="642"/>
+      <c r="F33" s="642"/>
+      <c r="G33" s="642"/>
+      <c r="H33" s="642"/>
+      <c r="I33" s="642"/>
+      <c r="J33" s="642"/>
+      <c r="K33" s="642"/>
+      <c r="L33" s="642"/>
     </row>
     <row r="34" spans="1:31" ht="27" customHeight="1" thickBot="1">
-      <c r="A34" s="682" t="s">
+      <c r="A34" s="645" t="s">
         <v>250</v>
       </c>
-      <c r="B34" s="683"/>
-      <c r="C34" s="683"/>
-      <c r="D34" s="683"/>
-      <c r="E34" s="683"/>
-      <c r="F34" s="683"/>
-      <c r="G34" s="683"/>
-      <c r="H34" s="683"/>
-      <c r="I34" s="683"/>
-      <c r="J34" s="683"/>
-      <c r="K34" s="683"/>
-      <c r="L34" s="684"/>
+      <c r="B34" s="646"/>
+      <c r="C34" s="646"/>
+      <c r="D34" s="646"/>
+      <c r="E34" s="646"/>
+      <c r="F34" s="646"/>
+      <c r="G34" s="646"/>
+      <c r="H34" s="646"/>
+      <c r="I34" s="646"/>
+      <c r="J34" s="646"/>
+      <c r="K34" s="646"/>
+      <c r="L34" s="647"/>
     </row>
     <row r="35" spans="1:31" ht="16.5" thickBot="1">
       <c r="A35" s="115"/>
@@ -7534,19 +7535,19 @@
         <v>24</v>
       </c>
       <c r="J36" s="17"/>
-      <c r="K36" s="671" t="s">
+      <c r="K36" s="665" t="s">
         <v>161</v>
       </c>
-      <c r="L36" s="664"/>
-      <c r="M36" s="664"/>
-      <c r="N36" s="664"/>
-      <c r="O36" s="664"/>
-      <c r="P36" s="664"/>
-      <c r="Q36" s="664"/>
-      <c r="R36" s="664"/>
-      <c r="S36" s="664"/>
-      <c r="T36" s="664"/>
-      <c r="U36" s="664"/>
+      <c r="L36" s="659"/>
+      <c r="M36" s="659"/>
+      <c r="N36" s="659"/>
+      <c r="O36" s="659"/>
+      <c r="P36" s="659"/>
+      <c r="Q36" s="659"/>
+      <c r="R36" s="659"/>
+      <c r="S36" s="659"/>
+      <c r="T36" s="659"/>
+      <c r="U36" s="659"/>
       <c r="V36" s="9"/>
       <c r="W36" s="29"/>
       <c r="X36" s="9"/>
@@ -7584,10 +7585,10 @@
       <c r="I37" s="81">
         <v>1</v>
       </c>
-      <c r="J37" s="691" t="s">
+      <c r="J37" s="657" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="671"/>
+      <c r="K37" s="665"/>
       <c r="N37" s="4"/>
       <c r="O37" s="6"/>
       <c r="R37" s="9"/>
@@ -7630,8 +7631,8 @@
       <c r="I38" s="81">
         <v>0</v>
       </c>
-      <c r="J38" s="692"/>
-      <c r="K38" s="671"/>
+      <c r="J38" s="658"/>
+      <c r="K38" s="665"/>
       <c r="N38" s="5"/>
       <c r="O38" s="6"/>
       <c r="R38" s="9"/>
@@ -7673,8 +7674,8 @@
       <c r="I39" s="81">
         <v>1</v>
       </c>
-      <c r="J39" s="692"/>
-      <c r="K39" s="671"/>
+      <c r="J39" s="658"/>
+      <c r="K39" s="665"/>
       <c r="N39" s="5"/>
       <c r="O39" s="6"/>
       <c r="R39" s="9"/>
@@ -7716,8 +7717,8 @@
       <c r="I40" s="81">
         <v>0</v>
       </c>
-      <c r="J40" s="692"/>
-      <c r="K40" s="671"/>
+      <c r="J40" s="658"/>
+      <c r="K40" s="665"/>
       <c r="N40" s="5"/>
       <c r="O40" s="6"/>
       <c r="R40" s="9"/>
@@ -7759,8 +7760,8 @@
       <c r="I41" s="81">
         <v>1</v>
       </c>
-      <c r="J41" s="692"/>
-      <c r="K41" s="671"/>
+      <c r="J41" s="658"/>
+      <c r="K41" s="665"/>
       <c r="N41" s="5"/>
       <c r="O41" s="6"/>
       <c r="R41" s="9"/>
@@ -7802,8 +7803,8 @@
       <c r="I42" s="81">
         <v>0</v>
       </c>
-      <c r="J42" s="692"/>
-      <c r="K42" s="671"/>
+      <c r="J42" s="658"/>
+      <c r="K42" s="665"/>
       <c r="N42" s="5"/>
       <c r="O42" s="6"/>
       <c r="R42" s="9"/>
@@ -7845,8 +7846,8 @@
       <c r="I43" s="81">
         <v>1</v>
       </c>
-      <c r="J43" s="692"/>
-      <c r="K43" s="671"/>
+      <c r="J43" s="658"/>
+      <c r="K43" s="665"/>
       <c r="N43" s="5"/>
       <c r="O43" s="6"/>
       <c r="R43" s="9"/>
@@ -7888,8 +7889,8 @@
       <c r="I44" s="81">
         <v>0</v>
       </c>
-      <c r="J44" s="692"/>
-      <c r="K44" s="671"/>
+      <c r="J44" s="658"/>
+      <c r="K44" s="665"/>
       <c r="N44" s="5"/>
       <c r="O44" s="6"/>
       <c r="R44" s="9"/>
@@ -7931,8 +7932,8 @@
       <c r="I45" s="81">
         <v>1</v>
       </c>
-      <c r="J45" s="692"/>
-      <c r="K45" s="671"/>
+      <c r="J45" s="658"/>
+      <c r="K45" s="665"/>
       <c r="N45" s="5"/>
       <c r="O45" s="6"/>
       <c r="R45" s="9"/>
@@ -7974,8 +7975,8 @@
       <c r="I46" s="81">
         <v>0</v>
       </c>
-      <c r="J46" s="692"/>
-      <c r="K46" s="671"/>
+      <c r="J46" s="658"/>
+      <c r="K46" s="665"/>
       <c r="N46" s="5"/>
       <c r="O46" s="6"/>
       <c r="R46" s="9"/>
@@ -8017,8 +8018,8 @@
       <c r="I47" s="81">
         <v>1</v>
       </c>
-      <c r="J47" s="692"/>
-      <c r="K47" s="671"/>
+      <c r="J47" s="658"/>
+      <c r="K47" s="665"/>
       <c r="N47" s="5"/>
       <c r="O47" s="6"/>
       <c r="R47" s="9"/>
@@ -8060,8 +8061,8 @@
       <c r="I48" s="81">
         <v>0</v>
       </c>
-      <c r="J48" s="692"/>
-      <c r="K48" s="671"/>
+      <c r="J48" s="658"/>
+      <c r="K48" s="665"/>
       <c r="N48" s="5"/>
       <c r="O48" s="6"/>
       <c r="R48" s="9"/>
@@ -8103,8 +8104,8 @@
       <c r="I49" s="81">
         <v>1</v>
       </c>
-      <c r="J49" s="692"/>
-      <c r="K49" s="671"/>
+      <c r="J49" s="658"/>
+      <c r="K49" s="665"/>
       <c r="N49" s="5"/>
       <c r="O49" s="6"/>
       <c r="X49" s="9"/>
@@ -8136,8 +8137,8 @@
       <c r="I50" s="81">
         <v>0</v>
       </c>
-      <c r="J50" s="692"/>
-      <c r="K50" s="671"/>
+      <c r="J50" s="658"/>
+      <c r="K50" s="665"/>
       <c r="N50" s="5"/>
       <c r="O50" s="6"/>
       <c r="X50" s="9"/>
@@ -8169,8 +8170,8 @@
       <c r="I51" s="81">
         <v>1</v>
       </c>
-      <c r="J51" s="692"/>
-      <c r="K51" s="671"/>
+      <c r="J51" s="658"/>
+      <c r="K51" s="665"/>
       <c r="N51" s="5"/>
       <c r="O51" s="6"/>
       <c r="X51" s="9"/>
@@ -8202,8 +8203,8 @@
       <c r="I52" s="81">
         <v>0</v>
       </c>
-      <c r="J52" s="692"/>
-      <c r="K52" s="671"/>
+      <c r="J52" s="658"/>
+      <c r="K52" s="665"/>
       <c r="N52" s="3"/>
       <c r="O52" s="6"/>
     </row>
@@ -8229,7 +8230,7 @@
         <v>21</v>
       </c>
       <c r="I53" s="128"/>
-      <c r="J53" s="686" t="s">
+      <c r="J53" s="651" t="s">
         <v>177</v>
       </c>
       <c r="K53" s="10"/>
@@ -8293,7 +8294,7 @@
         <v>25</v>
       </c>
       <c r="I54" s="81"/>
-      <c r="J54" s="687"/>
+      <c r="J54" s="652"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8">
         <v>0.5</v>
@@ -8359,7 +8360,7 @@
         <v>45</v>
       </c>
       <c r="I55" s="81"/>
-      <c r="J55" s="687"/>
+      <c r="J55" s="652"/>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
       <c r="M55" s="9"/>
@@ -8423,7 +8424,7 @@
         <v>46</v>
       </c>
       <c r="I56" s="81"/>
-      <c r="J56" s="687"/>
+      <c r="J56" s="652"/>
       <c r="K56" s="9"/>
       <c r="L56" s="10"/>
       <c r="M56" s="9"/>
@@ -8486,7 +8487,7 @@
         <v>47</v>
       </c>
       <c r="I57" s="81"/>
-      <c r="J57" s="687"/>
+      <c r="J57" s="652"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
       <c r="M57" s="9"/>
@@ -8549,7 +8550,7 @@
         <v>48</v>
       </c>
       <c r="I58" s="81"/>
-      <c r="J58" s="687"/>
+      <c r="J58" s="652"/>
       <c r="K58" s="10"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
@@ -8610,7 +8611,7 @@
         <v>49</v>
       </c>
       <c r="I59" s="81"/>
-      <c r="J59" s="687"/>
+      <c r="J59" s="652"/>
       <c r="K59" s="10"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -8672,7 +8673,7 @@
         <v>50</v>
       </c>
       <c r="I60" s="81"/>
-      <c r="J60" s="687"/>
+      <c r="J60" s="652"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -8733,7 +8734,7 @@
         <v>51</v>
       </c>
       <c r="I61" s="81"/>
-      <c r="J61" s="687"/>
+      <c r="J61" s="652"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
@@ -8794,7 +8795,7 @@
         <v>52</v>
       </c>
       <c r="I62" s="81"/>
-      <c r="J62" s="687"/>
+      <c r="J62" s="652"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -8854,7 +8855,7 @@
         <v>53</v>
       </c>
       <c r="I63" s="81"/>
-      <c r="J63" s="687"/>
+      <c r="J63" s="652"/>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
       <c r="M63" s="9"/>
@@ -8913,7 +8914,7 @@
         <v>54</v>
       </c>
       <c r="I64" s="81"/>
-      <c r="J64" s="687"/>
+      <c r="J64" s="652"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
@@ -8973,7 +8974,7 @@
         <v>55</v>
       </c>
       <c r="I65" s="81"/>
-      <c r="J65" s="687"/>
+      <c r="J65" s="652"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
@@ -9033,7 +9034,7 @@
         <v>56</v>
       </c>
       <c r="I66" s="81"/>
-      <c r="J66" s="687"/>
+      <c r="J66" s="652"/>
       <c r="K66" s="10"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
@@ -9092,7 +9093,7 @@
         <v>57</v>
       </c>
       <c r="I67" s="81"/>
-      <c r="J67" s="687"/>
+      <c r="J67" s="652"/>
       <c r="K67" s="10"/>
       <c r="L67" s="8"/>
       <c r="M67" s="9"/>
@@ -9151,7 +9152,7 @@
         <v>58</v>
       </c>
       <c r="I68" s="81"/>
-      <c r="J68" s="687"/>
+      <c r="J68" s="652"/>
       <c r="K68" s="9"/>
       <c r="L68" s="8"/>
       <c r="M68" s="9"/>
@@ -9211,7 +9212,7 @@
         <v>59</v>
       </c>
       <c r="I69" s="81"/>
-      <c r="J69" s="687"/>
+      <c r="J69" s="652"/>
       <c r="K69" s="9"/>
       <c r="L69" s="8"/>
       <c r="M69" s="9"/>
@@ -9270,7 +9271,7 @@
         <v>60</v>
       </c>
       <c r="I70" s="81"/>
-      <c r="J70" s="687"/>
+      <c r="J70" s="652"/>
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
       <c r="M70" s="9"/>
@@ -10155,24 +10156,24 @@
       <c r="I85" s="23"/>
       <c r="J85" s="7"/>
       <c r="K85" s="9"/>
-      <c r="L85" s="685"/>
-      <c r="M85" s="685"/>
-      <c r="N85" s="685">
-        <v>0</v>
-      </c>
-      <c r="O85" s="685">
-        <v>0</v>
-      </c>
-      <c r="P85" s="685">
-        <v>0</v>
-      </c>
-      <c r="Q85" s="685">
-        <v>0</v>
-      </c>
-      <c r="R85" s="685">
-        <v>0</v>
-      </c>
-      <c r="S85" s="685">
+      <c r="L85" s="650"/>
+      <c r="M85" s="650"/>
+      <c r="N85" s="650">
+        <v>0</v>
+      </c>
+      <c r="O85" s="650">
+        <v>0</v>
+      </c>
+      <c r="P85" s="650">
+        <v>0</v>
+      </c>
+      <c r="Q85" s="650">
+        <v>0</v>
+      </c>
+      <c r="R85" s="650">
+        <v>0</v>
+      </c>
+      <c r="S85" s="650">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -10189,7 +10190,7 @@
       <c r="AF86" s="167"/>
     </row>
     <row r="87" spans="1:32" ht="15.75">
-      <c r="A87" s="689" t="s">
+      <c r="A87" s="654" t="s">
         <v>87</v>
       </c>
       <c r="B87" s="63" t="s">
@@ -10221,7 +10222,7 @@
       <c r="AF87" s="167"/>
     </row>
     <row r="88" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A88" s="669"/>
+      <c r="A88" s="655"/>
       <c r="B88" s="19">
         <v>0</v>
       </c>
@@ -10245,12 +10246,12 @@
         <v>0</v>
       </c>
       <c r="J88" s="58"/>
-      <c r="K88" s="688" t="s">
+      <c r="K88" s="653" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:32" ht="15.75" customHeight="1">
-      <c r="A89" s="669"/>
+      <c r="A89" s="655"/>
       <c r="B89" s="19">
         <v>0</v>
       </c>
@@ -10274,14 +10275,14 @@
         <v>4</v>
       </c>
       <c r="J89" s="13"/>
-      <c r="K89" s="688"/>
+      <c r="K89" s="653"/>
       <c r="L89" s="56"/>
       <c r="N89" s="11"/>
       <c r="O89" s="6"/>
       <c r="S89" s="32"/>
     </row>
     <row r="90" spans="1:32" ht="15.75">
-      <c r="A90" s="669"/>
+      <c r="A90" s="655"/>
       <c r="B90" s="19">
         <v>0</v>
       </c>
@@ -10305,14 +10306,14 @@
         <v>2</v>
       </c>
       <c r="J90" s="13"/>
-      <c r="K90" s="688"/>
+      <c r="K90" s="653"/>
       <c r="L90" s="56"/>
       <c r="N90" s="11"/>
       <c r="O90" s="6"/>
       <c r="S90" s="32"/>
     </row>
     <row r="91" spans="1:32" ht="15.75">
-      <c r="A91" s="669"/>
+      <c r="A91" s="655"/>
       <c r="B91" s="19">
         <v>0</v>
       </c>
@@ -10336,14 +10337,14 @@
         <v>6</v>
       </c>
       <c r="J91" s="13"/>
-      <c r="K91" s="688"/>
+      <c r="K91" s="653"/>
       <c r="L91" s="56"/>
       <c r="N91" s="11"/>
       <c r="O91" s="6"/>
       <c r="S91" s="32"/>
     </row>
     <row r="92" spans="1:32" ht="15.75">
-      <c r="A92" s="669"/>
+      <c r="A92" s="655"/>
       <c r="B92" s="19">
         <v>0</v>
       </c>
@@ -10367,14 +10368,14 @@
         <v>1</v>
       </c>
       <c r="J92" s="13"/>
-      <c r="K92" s="688"/>
+      <c r="K92" s="653"/>
       <c r="L92" s="56"/>
       <c r="N92" s="11"/>
       <c r="O92" s="6"/>
       <c r="S92" s="32"/>
     </row>
     <row r="93" spans="1:32" ht="15.75">
-      <c r="A93" s="669"/>
+      <c r="A93" s="655"/>
       <c r="B93" s="19">
         <v>0</v>
       </c>
@@ -10398,14 +10399,14 @@
         <v>5</v>
       </c>
       <c r="J93" s="13"/>
-      <c r="K93" s="688"/>
+      <c r="K93" s="653"/>
       <c r="L93" s="56"/>
       <c r="N93" s="11"/>
       <c r="O93" s="6"/>
       <c r="S93" s="32"/>
     </row>
     <row r="94" spans="1:32" ht="15.75">
-      <c r="A94" s="669"/>
+      <c r="A94" s="655"/>
       <c r="B94" s="19">
         <v>0</v>
       </c>
@@ -10429,14 +10430,14 @@
         <v>3</v>
       </c>
       <c r="J94" s="13"/>
-      <c r="K94" s="688"/>
+      <c r="K94" s="653"/>
       <c r="L94" s="56"/>
       <c r="N94" s="11"/>
       <c r="O94" s="6"/>
       <c r="S94" s="32"/>
     </row>
     <row r="95" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A95" s="669"/>
+      <c r="A95" s="655"/>
       <c r="B95" s="19">
         <v>0</v>
       </c>
@@ -10460,14 +10461,14 @@
         <v>7</v>
       </c>
       <c r="J95" s="13"/>
-      <c r="K95" s="688"/>
+      <c r="K95" s="653"/>
       <c r="L95" s="56"/>
       <c r="N95" s="11"/>
       <c r="O95" s="6"/>
       <c r="S95" s="32"/>
     </row>
     <row r="96" spans="1:32" ht="15.75">
-      <c r="A96" s="669"/>
+      <c r="A96" s="655"/>
       <c r="B96" s="19">
         <v>1</v>
       </c>
@@ -10493,14 +10494,14 @@
       <c r="J96" s="148">
         <v>13.6</v>
       </c>
-      <c r="K96" s="688"/>
+      <c r="K96" s="653"/>
       <c r="L96" s="56"/>
       <c r="N96" s="11"/>
       <c r="O96" s="6"/>
       <c r="S96" s="32"/>
     </row>
     <row r="97" spans="1:19" ht="15.75">
-      <c r="A97" s="669"/>
+      <c r="A97" s="655"/>
       <c r="B97" s="19">
         <v>1</v>
       </c>
@@ -10524,14 +10525,14 @@
         <v>4</v>
       </c>
       <c r="J97" s="13"/>
-      <c r="K97" s="688"/>
+      <c r="K97" s="653"/>
       <c r="L97" s="56"/>
       <c r="N97" s="11"/>
       <c r="O97" s="6"/>
       <c r="S97" s="32"/>
     </row>
     <row r="98" spans="1:19" ht="15.75">
-      <c r="A98" s="669"/>
+      <c r="A98" s="655"/>
       <c r="B98" s="19">
         <v>1</v>
       </c>
@@ -10555,14 +10556,14 @@
         <v>2</v>
       </c>
       <c r="J98" s="13"/>
-      <c r="K98" s="688"/>
+      <c r="K98" s="653"/>
       <c r="L98" s="56"/>
       <c r="N98" s="11"/>
       <c r="O98" s="6"/>
       <c r="S98" s="32"/>
     </row>
     <row r="99" spans="1:19" ht="15.75">
-      <c r="A99" s="669"/>
+      <c r="A99" s="655"/>
       <c r="B99" s="19">
         <v>1</v>
       </c>
@@ -10586,14 +10587,14 @@
         <v>6</v>
       </c>
       <c r="J99" s="13"/>
-      <c r="K99" s="688"/>
+      <c r="K99" s="653"/>
       <c r="L99" s="56"/>
       <c r="N99" s="11"/>
       <c r="O99" s="6"/>
       <c r="S99" s="32"/>
     </row>
     <row r="100" spans="1:19" ht="15.75">
-      <c r="A100" s="669"/>
+      <c r="A100" s="655"/>
       <c r="B100" s="19">
         <v>1</v>
       </c>
@@ -10617,14 +10618,14 @@
         <v>1</v>
       </c>
       <c r="J100" s="13"/>
-      <c r="K100" s="688"/>
+      <c r="K100" s="653"/>
       <c r="L100" s="56"/>
       <c r="N100" s="11"/>
       <c r="O100" s="6"/>
       <c r="S100" s="32"/>
     </row>
     <row r="101" spans="1:19" ht="15.75">
-      <c r="A101" s="669"/>
+      <c r="A101" s="655"/>
       <c r="B101" s="19">
         <v>1</v>
       </c>
@@ -10648,14 +10649,14 @@
         <v>5</v>
       </c>
       <c r="J101" s="13"/>
-      <c r="K101" s="688"/>
+      <c r="K101" s="653"/>
       <c r="L101" s="56"/>
       <c r="N101" s="11"/>
       <c r="O101" s="6"/>
       <c r="S101" s="32"/>
     </row>
     <row r="102" spans="1:19" ht="15.75">
-      <c r="A102" s="669"/>
+      <c r="A102" s="655"/>
       <c r="B102" s="19">
         <v>1</v>
       </c>
@@ -10679,14 +10680,14 @@
         <v>3</v>
       </c>
       <c r="J102" s="13"/>
-      <c r="K102" s="688"/>
+      <c r="K102" s="653"/>
       <c r="L102" s="56"/>
       <c r="N102" s="11"/>
       <c r="O102" s="6"/>
       <c r="S102" s="32"/>
     </row>
     <row r="103" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A103" s="669"/>
+      <c r="A103" s="655"/>
       <c r="B103" s="19">
         <v>1</v>
       </c>
@@ -10710,14 +10711,14 @@
         <v>7</v>
       </c>
       <c r="J103" s="13"/>
-      <c r="K103" s="688"/>
+      <c r="K103" s="653"/>
       <c r="L103" s="56"/>
       <c r="N103" s="11"/>
       <c r="O103" s="6"/>
       <c r="S103" s="32"/>
     </row>
     <row r="104" spans="1:19" ht="15.75">
-      <c r="A104" s="669"/>
+      <c r="A104" s="655"/>
       <c r="B104" s="132" t="s">
         <v>149</v>
       </c>
@@ -10745,7 +10746,7 @@
       <c r="S104" s="32"/>
     </row>
     <row r="105" spans="1:19" ht="15.75">
-      <c r="A105" s="669"/>
+      <c r="A105" s="655"/>
       <c r="B105" s="19">
         <v>0</v>
       </c>
@@ -10769,7 +10770,7 @@
       <c r="J105" s="146">
         <v>1</v>
       </c>
-      <c r="K105" s="675" t="s">
+      <c r="K105" s="638" t="s">
         <v>159</v>
       </c>
       <c r="L105" s="2" t="s">
@@ -10779,7 +10780,7 @@
       <c r="S105" s="32"/>
     </row>
     <row r="106" spans="1:19" ht="15.75">
-      <c r="A106" s="669"/>
+      <c r="A106" s="655"/>
       <c r="B106" s="19">
         <v>0</v>
       </c>
@@ -10803,7 +10804,7 @@
       <c r="J106" s="146">
         <v>0.99719999999999998</v>
       </c>
-      <c r="K106" s="675"/>
+      <c r="K106" s="638"/>
       <c r="L106" t="s">
         <v>157</v>
       </c>
@@ -10812,7 +10813,7 @@
       <c r="S106" s="32"/>
     </row>
     <row r="107" spans="1:19" ht="15.75">
-      <c r="A107" s="669"/>
+      <c r="A107" s="655"/>
       <c r="B107" s="19">
         <v>0</v>
       </c>
@@ -10836,14 +10837,14 @@
       <c r="J107" s="146">
         <v>0.99429999999999996</v>
       </c>
-      <c r="K107" s="675"/>
+      <c r="K107" s="638"/>
       <c r="L107" s="12"/>
       <c r="O107" s="6"/>
       <c r="Q107" s="11"/>
       <c r="S107" s="32"/>
     </row>
     <row r="108" spans="1:19" ht="15.75">
-      <c r="A108" s="669"/>
+      <c r="A108" s="655"/>
       <c r="B108" s="19">
         <v>0</v>
       </c>
@@ -10867,14 +10868,14 @@
       <c r="J108" s="3">
         <v>0.99139999999999995</v>
       </c>
-      <c r="K108" s="675"/>
+      <c r="K108" s="638"/>
       <c r="L108" s="12"/>
       <c r="O108" s="6"/>
       <c r="Q108" s="11"/>
       <c r="S108" s="32"/>
     </row>
     <row r="109" spans="1:19" ht="15.75">
-      <c r="A109" s="669"/>
+      <c r="A109" s="655"/>
       <c r="B109" s="19">
         <v>0</v>
       </c>
@@ -10898,14 +10899,14 @@
       <c r="J109" s="3">
         <v>0.98850000000000005</v>
       </c>
-      <c r="K109" s="675"/>
+      <c r="K109" s="638"/>
       <c r="L109" s="12"/>
       <c r="O109" s="6"/>
       <c r="Q109" s="11"/>
       <c r="S109" s="32"/>
     </row>
     <row r="110" spans="1:19" ht="15.75">
-      <c r="A110" s="669"/>
+      <c r="A110" s="655"/>
       <c r="B110" s="19">
         <v>0</v>
       </c>
@@ -10929,14 +10930,14 @@
       <c r="J110" s="3">
         <v>0.98560000000000003</v>
       </c>
-      <c r="K110" s="675"/>
+      <c r="K110" s="638"/>
       <c r="L110" s="57"/>
       <c r="O110" s="6"/>
       <c r="Q110" s="11"/>
       <c r="S110" s="32"/>
     </row>
     <row r="111" spans="1:19" ht="15.75">
-      <c r="A111" s="669"/>
+      <c r="A111" s="655"/>
       <c r="B111" s="19">
         <v>0</v>
       </c>
@@ -10960,14 +10961,14 @@
       <c r="J111" s="3">
         <v>0.98260000000000003</v>
       </c>
-      <c r="K111" s="675"/>
+      <c r="K111" s="638"/>
       <c r="L111" s="12"/>
       <c r="O111" s="6"/>
       <c r="Q111" s="11"/>
       <c r="S111" s="32"/>
     </row>
     <row r="112" spans="1:19" ht="15.75">
-      <c r="A112" s="669"/>
+      <c r="A112" s="655"/>
       <c r="B112" s="19">
         <v>0</v>
       </c>
@@ -10991,14 +10992,14 @@
       <c r="J112" s="147">
         <v>0.9798</v>
       </c>
-      <c r="K112" s="675"/>
+      <c r="K112" s="638"/>
       <c r="L112" s="12"/>
       <c r="O112" s="6"/>
       <c r="Q112" s="11"/>
       <c r="S112" s="32"/>
     </row>
     <row r="113" spans="1:19" ht="15.75">
-      <c r="A113" s="669"/>
+      <c r="A113" s="655"/>
       <c r="B113" s="19">
         <v>1</v>
       </c>
@@ -11022,14 +11023,14 @@
       <c r="J113" s="147">
         <v>1.0233000000000001</v>
       </c>
-      <c r="K113" s="675"/>
+      <c r="K113" s="638"/>
       <c r="L113" s="12"/>
       <c r="O113" s="6"/>
       <c r="Q113" s="11"/>
       <c r="S113" s="32"/>
     </row>
     <row r="114" spans="1:19" ht="15.75">
-      <c r="A114" s="669"/>
+      <c r="A114" s="655"/>
       <c r="B114" s="19">
         <v>1</v>
       </c>
@@ -11053,14 +11054,14 @@
       <c r="J114" s="3">
         <v>1.0204</v>
       </c>
-      <c r="K114" s="675"/>
+      <c r="K114" s="638"/>
       <c r="L114" s="12"/>
       <c r="O114" s="6"/>
       <c r="Q114" s="11"/>
       <c r="S114" s="32"/>
     </row>
     <row r="115" spans="1:19" ht="15.75">
-      <c r="A115" s="669"/>
+      <c r="A115" s="655"/>
       <c r="B115" s="19">
         <v>1</v>
       </c>
@@ -11084,14 +11085,14 @@
       <c r="J115" s="3">
         <v>1.0175000000000001</v>
       </c>
-      <c r="K115" s="675"/>
+      <c r="K115" s="638"/>
       <c r="L115" s="12"/>
       <c r="O115" s="6"/>
       <c r="Q115" s="11"/>
       <c r="S115" s="32"/>
     </row>
     <row r="116" spans="1:19" ht="15.75">
-      <c r="A116" s="669"/>
+      <c r="A116" s="655"/>
       <c r="B116" s="19">
         <v>1</v>
       </c>
@@ -11115,14 +11116,14 @@
       <c r="J116" s="3">
         <v>1.0145999999999999</v>
       </c>
-      <c r="K116" s="675"/>
+      <c r="K116" s="638"/>
       <c r="L116" s="57"/>
       <c r="O116" s="6"/>
       <c r="Q116" s="11"/>
       <c r="S116" s="32"/>
     </row>
     <row r="117" spans="1:19" ht="15.75">
-      <c r="A117" s="669"/>
+      <c r="A117" s="655"/>
       <c r="B117" s="19">
         <v>1</v>
       </c>
@@ -11146,14 +11147,14 @@
       <c r="J117" s="3">
         <v>1.0117</v>
       </c>
-      <c r="K117" s="675"/>
+      <c r="K117" s="638"/>
       <c r="L117" s="12"/>
       <c r="O117" s="6"/>
       <c r="Q117" s="11"/>
       <c r="S117" s="32"/>
     </row>
     <row r="118" spans="1:19" ht="15.75">
-      <c r="A118" s="669"/>
+      <c r="A118" s="655"/>
       <c r="B118" s="19">
         <v>1</v>
       </c>
@@ -11177,14 +11178,14 @@
       <c r="J118" s="3">
         <v>1.0087999999999999</v>
       </c>
-      <c r="K118" s="675"/>
+      <c r="K118" s="638"/>
       <c r="L118" s="12"/>
       <c r="O118" s="6"/>
       <c r="Q118" s="11"/>
       <c r="S118" s="32"/>
     </row>
     <row r="119" spans="1:19" ht="15.75">
-      <c r="A119" s="669"/>
+      <c r="A119" s="655"/>
       <c r="B119" s="19">
         <v>1</v>
       </c>
@@ -11208,14 +11209,14 @@
       <c r="J119" s="3">
         <v>1.0059</v>
       </c>
-      <c r="K119" s="675"/>
+      <c r="K119" s="638"/>
       <c r="L119" s="12"/>
       <c r="O119" s="6"/>
       <c r="Q119" s="11"/>
       <c r="S119" s="32"/>
     </row>
     <row r="120" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A120" s="690"/>
+      <c r="A120" s="656"/>
       <c r="B120" s="22">
         <v>1</v>
       </c>
@@ -11239,7 +11240,7 @@
       <c r="J120" s="142">
         <v>1.0029999999999999</v>
       </c>
-      <c r="K120" s="675"/>
+      <c r="K120" s="638"/>
       <c r="L120" s="12"/>
       <c r="O120" s="6"/>
       <c r="Q120" s="11"/>
@@ -11846,6 +11847,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="L36:U36"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="K36:K52"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="K105:K120"/>
     <mergeCell ref="H6:H9"/>
@@ -11862,25 +11882,6 @@
     <mergeCell ref="K88:K103"/>
     <mergeCell ref="A87:A120"/>
     <mergeCell ref="J37:J52"/>
-    <mergeCell ref="L36:U36"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="K36:K52"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26355,9 +26356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="9" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF52" sqref="AF22:AF52"/>
+      <selection pane="topRight" activeCell="AG90" sqref="AG90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -26538,7 +26539,7 @@
       <c r="I4" s="308">
         <v>1</v>
       </c>
-      <c r="J4" s="691" t="s">
+      <c r="J4" s="657" t="s">
         <v>256</v>
       </c>
       <c r="K4" s="354">
@@ -26654,7 +26655,7 @@
       <c r="I5" s="308">
         <v>0</v>
       </c>
-      <c r="J5" s="691"/>
+      <c r="J5" s="657"/>
       <c r="K5" s="354">
         <v>0.02</v>
       </c>
@@ -26720,7 +26721,7 @@
         <v>0.14100350838113279</v>
       </c>
       <c r="AF5" s="371">
-        <f t="shared" ref="AF5:AF19" si="7">AG5*1.5</f>
+        <f t="shared" ref="AF5:AF18" si="7">AG5*1.5</f>
         <v>0.21197411886552942</v>
       </c>
       <c r="AG5" s="370">
@@ -26767,7 +26768,7 @@
       <c r="I6" s="308">
         <v>1</v>
       </c>
-      <c r="J6" s="691"/>
+      <c r="J6" s="657"/>
       <c r="K6" s="354">
         <v>0.03</v>
       </c>
@@ -26880,7 +26881,7 @@
       <c r="I7" s="308">
         <v>0</v>
       </c>
-      <c r="J7" s="691"/>
+      <c r="J7" s="657"/>
       <c r="K7" s="354">
         <v>0.04</v>
       </c>
@@ -26993,7 +26994,7 @@
       <c r="I8" s="308">
         <v>1</v>
       </c>
-      <c r="J8" s="691"/>
+      <c r="J8" s="657"/>
       <c r="K8" s="354">
         <v>0.05</v>
       </c>
@@ -27106,7 +27107,7 @@
       <c r="I9" s="308">
         <v>0</v>
       </c>
-      <c r="J9" s="691"/>
+      <c r="J9" s="657"/>
       <c r="K9" s="354">
         <v>0.06</v>
       </c>
@@ -27219,7 +27220,7 @@
       <c r="I10" s="308">
         <v>1</v>
       </c>
-      <c r="J10" s="691"/>
+      <c r="J10" s="657"/>
       <c r="K10" s="354">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -27332,7 +27333,7 @@
       <c r="I11" s="614">
         <v>0</v>
       </c>
-      <c r="J11" s="691"/>
+      <c r="J11" s="657"/>
       <c r="K11" s="354">
         <v>0.08</v>
       </c>
@@ -27445,7 +27446,7 @@
       <c r="I12" s="308">
         <v>1</v>
       </c>
-      <c r="J12" s="691"/>
+      <c r="J12" s="657"/>
       <c r="K12" s="354">
         <v>0.09</v>
       </c>
@@ -27558,7 +27559,7 @@
       <c r="I13" s="308">
         <v>0</v>
       </c>
-      <c r="J13" s="691"/>
+      <c r="J13" s="657"/>
       <c r="K13" s="354">
         <v>0.1</v>
       </c>
@@ -27671,7 +27672,7 @@
       <c r="I14" s="308">
         <v>1</v>
       </c>
-      <c r="J14" s="691"/>
+      <c r="J14" s="657"/>
       <c r="K14" s="354">
         <v>0.11</v>
       </c>
@@ -27784,7 +27785,7 @@
       <c r="I15" s="614">
         <v>0</v>
       </c>
-      <c r="J15" s="691"/>
+      <c r="J15" s="657"/>
       <c r="K15" s="354">
         <v>0.12</v>
       </c>
@@ -27897,7 +27898,7 @@
       <c r="I16" s="308">
         <v>1</v>
       </c>
-      <c r="J16" s="691"/>
+      <c r="J16" s="657"/>
       <c r="K16" s="354">
         <v>0.13</v>
       </c>
@@ -28011,7 +28012,7 @@
       <c r="I17" s="614">
         <v>0</v>
       </c>
-      <c r="J17" s="691"/>
+      <c r="J17" s="657"/>
       <c r="K17" s="354">
         <v>0.14000000000000001</v>
       </c>
@@ -28124,7 +28125,7 @@
       <c r="I18" s="614">
         <v>1</v>
       </c>
-      <c r="J18" s="691"/>
+      <c r="J18" s="657"/>
       <c r="K18" s="354">
         <v>0.15</v>
       </c>
@@ -28234,7 +28235,7 @@
       <c r="I19" s="308">
         <v>0</v>
       </c>
-      <c r="J19" s="691"/>
+      <c r="J19" s="657"/>
       <c r="K19" s="354">
         <v>0.16</v>
       </c>
@@ -31769,6 +31770,9 @@
         <f>AVERAGE(N55,Q55,T55,W55,Z55,AC55)</f>
         <v>1</v>
       </c>
+      <c r="AH55" s="5">
+        <v>0</v>
+      </c>
       <c r="AI55" s="335">
         <v>0</v>
       </c>
@@ -31869,6 +31873,9 @@
         <f t="shared" ref="AG56:AG70" si="25">AVERAGE(N56,Q56,T56,W56,Z56,AC56)</f>
         <v>0.98939995367301148</v>
       </c>
+      <c r="AH56" s="605">
+        <v>1</v>
+      </c>
       <c r="AI56" s="599">
         <v>-1.0524209683873544E-2</v>
       </c>
@@ -31969,6 +31976,9 @@
         <f t="shared" si="25"/>
         <v>0.97870009550853476</v>
       </c>
+      <c r="AH57" s="605">
+        <v>2</v>
+      </c>
       <c r="AI57" s="599">
         <v>-2.1128451380552204E-2</v>
       </c>
@@ -32069,6 +32079,9 @@
         <f t="shared" si="25"/>
         <v>0.96779962362987881</v>
       </c>
+      <c r="AH58" s="5">
+        <v>3</v>
+      </c>
       <c r="AI58" s="339">
         <v>-3.1772709083633506E-2</v>
       </c>
@@ -32169,6 +32182,9 @@
         <f t="shared" si="25"/>
         <v>0.95682519681536549</v>
       </c>
+      <c r="AH59" s="605">
+        <v>4</v>
+      </c>
       <c r="AI59" s="599">
         <v>-4.2416966786714812E-2</v>
       </c>
@@ -32269,6 +32285,9 @@
         <f t="shared" si="25"/>
         <v>0.9460199477918686</v>
       </c>
+      <c r="AH60" s="605">
+        <v>5</v>
+      </c>
       <c r="AI60" s="339">
         <v>-5.3021208483393471E-2</v>
       </c>
@@ -32369,6 +32388,9 @@
         <f t="shared" si="25"/>
         <v>0.93495899370953495</v>
       </c>
+      <c r="AH61" s="5">
+        <v>6</v>
+      </c>
       <c r="AI61" s="339">
         <v>-6.3625450180072124E-2</v>
       </c>
@@ -32469,6 +32491,9 @@
         <f t="shared" si="25"/>
         <v>0.92385130661693504</v>
       </c>
+      <c r="AH62" s="605">
+        <v>7</v>
+      </c>
       <c r="AI62" s="339">
         <v>-7.4029611844737914E-2</v>
       </c>
@@ -32567,6 +32592,9 @@
       <c r="AG63" s="606">
         <f t="shared" si="25"/>
         <v>1.0827186302686815</v>
+      </c>
+      <c r="AH63" s="605">
+        <v>8</v>
       </c>
       <c r="AI63" s="599">
         <v>8.2032813125250126E-2</v>
@@ -32664,6 +32692,9 @@
         <f t="shared" si="25"/>
         <v>1.0726595815894693</v>
       </c>
+      <c r="AH64" s="5">
+        <v>9</v>
+      </c>
       <c r="AI64" s="339">
         <v>7.2428971588635468E-2</v>
       </c>
@@ -32760,6 +32791,9 @@
         <f t="shared" si="25"/>
         <v>1.0626148078446687</v>
       </c>
+      <c r="AH65" s="605">
+        <v>10</v>
+      </c>
       <c r="AI65" s="339">
         <v>6.2264905962384848E-2</v>
       </c>
@@ -32856,6 +32890,9 @@
         <f t="shared" si="25"/>
         <v>1.0523160893490928</v>
       </c>
+      <c r="AH66" s="605">
+        <v>11</v>
+      </c>
       <c r="AI66" s="339">
         <v>5.2020808323329289E-2</v>
       </c>
@@ -32952,6 +32989,9 @@
         <f t="shared" si="25"/>
         <v>1.0420157098013625</v>
       </c>
+      <c r="AH67" s="5">
+        <v>12</v>
+      </c>
       <c r="AI67" s="339">
         <v>4.1816726690676195E-2</v>
       </c>
@@ -33048,6 +33088,9 @@
         <f t="shared" si="25"/>
         <v>1.0316226676090801</v>
       </c>
+      <c r="AH68" s="605">
+        <v>13</v>
+      </c>
       <c r="AI68" s="339">
         <v>3.1452581032412878E-2</v>
       </c>
@@ -33144,6 +33187,9 @@
         <f t="shared" si="25"/>
         <v>1.021217343130661</v>
       </c>
+      <c r="AH69" s="605">
+        <v>14</v>
+      </c>
       <c r="AI69" s="339">
         <v>2.1048419367747088E-2</v>
       </c>
@@ -33239,6 +33285,9 @@
       <c r="AG70" s="594">
         <f t="shared" si="25"/>
         <v>1.0106715008575424</v>
+      </c>
+      <c r="AH70" s="5">
+        <v>15</v>
       </c>
       <c r="AI70" s="339">
         <v>1.0564225690276013E-2</v>
@@ -33366,6 +33415,9 @@
         <f>AVERAGE(N72,Q72,T72,W72,Z72,AC72)</f>
         <v>1</v>
       </c>
+      <c r="AH72" s="5">
+        <v>0</v>
+      </c>
       <c r="AI72" s="335">
         <v>0</v>
       </c>
@@ -33462,6 +33514,9 @@
         <f t="shared" ref="AG73:AG87" si="38">AVERAGE(N73,Q73,T73,W73,Z73,AC73)</f>
         <v>0.99717461176181799</v>
       </c>
+      <c r="AH73" s="619">
+        <v>1</v>
+      </c>
       <c r="AI73" s="612">
         <v>-2.8000000000000247E-3</v>
       </c>
@@ -33558,6 +33613,9 @@
         <f t="shared" si="38"/>
         <v>0.99432305875801585</v>
       </c>
+      <c r="AH74" s="5">
+        <v>2</v>
+      </c>
       <c r="AI74" s="612">
         <v>-5.7000000000000384E-3</v>
       </c>
@@ -33653,6 +33711,9 @@
         <f t="shared" si="38"/>
         <v>0.99140215918860575</v>
       </c>
+      <c r="AH75" s="619">
+        <v>3</v>
+      </c>
       <c r="AI75" s="339">
         <v>-8.600000000000052E-3</v>
       </c>
@@ -33749,6 +33810,9 @@
         <f t="shared" si="38"/>
         <v>0.98845268871874314</v>
       </c>
+      <c r="AH76" s="5">
+        <v>4</v>
+      </c>
       <c r="AI76" s="612">
         <v>-1.1499999999999955E-2</v>
       </c>
@@ -33844,6 +33908,9 @@
         <f t="shared" si="38"/>
         <v>0.98562776088527071</v>
       </c>
+      <c r="AH77" s="619">
+        <v>5</v>
+      </c>
       <c r="AI77" s="339">
         <v>-1.4399999999999968E-2</v>
       </c>
@@ -33939,6 +34006,9 @@
         <f t="shared" si="38"/>
         <v>0.98280861965893129</v>
       </c>
+      <c r="AH78" s="5">
+        <v>6</v>
+      </c>
       <c r="AI78" s="339">
         <v>-1.7399999999999971E-2</v>
       </c>
@@ -34034,6 +34104,9 @@
         <f t="shared" si="38"/>
         <v>0.98003123080023602</v>
       </c>
+      <c r="AH79" s="619">
+        <v>7</v>
+      </c>
       <c r="AI79" s="339">
         <v>-2.0199999999999996E-2</v>
       </c>
@@ -34130,6 +34203,9 @@
         <f t="shared" si="38"/>
         <v>1.0239280239047532</v>
       </c>
+      <c r="AH80" s="5">
+        <v>8</v>
+      </c>
       <c r="AI80" s="612">
         <v>2.3300000000000098E-2</v>
       </c>
@@ -34225,6 +34301,9 @@
         <f t="shared" si="38"/>
         <v>1.0209940166804954</v>
       </c>
+      <c r="AH81" s="619">
+        <v>9</v>
+      </c>
       <c r="AI81" s="339">
         <v>2.0399999999999974E-2</v>
       </c>
@@ -34320,6 +34399,9 @@
         <f t="shared" si="38"/>
         <v>1.0179751415776905</v>
       </c>
+      <c r="AH82" s="5">
+        <v>10</v>
+      </c>
       <c r="AI82" s="339">
         <v>1.7500000000000071E-2</v>
       </c>
@@ -34415,6 +34497,9 @@
         <f t="shared" si="38"/>
         <v>1.0147889471244553</v>
       </c>
+      <c r="AH83" s="619">
+        <v>11</v>
+      </c>
       <c r="AI83" s="339">
         <v>1.4599999999999946E-2</v>
       </c>
@@ -34510,6 +34595,9 @@
         <f t="shared" si="38"/>
         <v>1.011916687738043</v>
       </c>
+      <c r="AH84" s="5">
+        <v>12</v>
+      </c>
       <c r="AI84" s="339">
         <v>1.1700000000000044E-2</v>
       </c>
@@ -34605,6 +34693,9 @@
         <f t="shared" si="38"/>
         <v>1.0088917351317892</v>
       </c>
+      <c r="AH85" s="619">
+        <v>13</v>
+      </c>
       <c r="AI85" s="339">
         <v>8.799999999999919E-3</v>
       </c>
@@ -34700,6 +34791,9 @@
         <f t="shared" si="38"/>
         <v>1.0059724501121314</v>
       </c>
+      <c r="AH86" s="5">
+        <v>14</v>
+      </c>
       <c r="AI86" s="339">
         <v>5.9000000000000163E-3</v>
       </c>
@@ -34794,6 +34888,9 @@
       <c r="AG87" s="594">
         <f t="shared" si="38"/>
         <v>1.0030668094445463</v>
+      </c>
+      <c r="AH87" s="619">
+        <v>15</v>
       </c>
       <c r="AI87" s="352">
         <v>2.9999999999998916E-3</v>
@@ -34837,12 +34934,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet4!F11:F11</xm:f>
-              <xm:sqref>BE22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet4!F12:F12</xm:f>
-              <xm:sqref>BE23</xm:sqref>
+              <xm:f>Sheet4!F11:F12</xm:f>
+              <xm:sqref>BA39</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -34857,8 +34950,12 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet4!F11:F12</xm:f>
-              <xm:sqref>BA39</xm:sqref>
+              <xm:f>Sheet4!F11:F11</xm:f>
+              <xm:sqref>BE22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet4!F12:F12</xm:f>
+              <xm:sqref>BE23</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -41050,6 +41147,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:D6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:D10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:D14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:D18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:D22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:D26"/>
     <mergeCell ref="B39:B42"/>
@@ -41060,17 +41168,6 @@
     <mergeCell ref="C31:D34"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="C35:D38"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:D14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:D18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:D22"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:D6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>